<commit_message>
generate data set api added
</commit_message>
<xml_diff>
--- a/integration/speed_at_intersection.xlsx
+++ b/integration/speed_at_intersection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ReachIntersection" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="SpeedAtIntersection" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="SetFinalSpeed" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReachIntersection" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpeedAtIntersection" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SetFinalSpeed" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="A2:D11"/>
@@ -607,6 +607,182 @@
       <c r="D8" t="inlineStr">
         <is>
           <t>15</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1165.492770458883</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>-666.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>740</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1165.492770458883</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>-1687.7</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>-5271</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1609.0</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>4060.344</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>956.795</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>133.57108176521356</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>1730</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>956.795</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2174.030431</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4388</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>956.795</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>956.795</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>4388</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>-1239.0</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>-1123.5137</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>-680</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>133.5711</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>847.418</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -621,7 +797,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -864,6 +1040,193 @@
       <c r="C14" t="inlineStr">
         <is>
           <t>-380.68</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>-1900</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>4544.8</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4544.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>-1900</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>-3119.4</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>-4406.942272</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1227.23</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1227.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1227.23</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1227.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>-853</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>526.0</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>240.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>-2261</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>526.0</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>-2255.709063</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2419</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>228.201385</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1501.4845</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>-70</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>956.795</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>-663.4069</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>-70</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>-1518.0</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>-1518.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>-70</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>1076.1574168684874</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1076.1574168684874</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>-70</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>1432.45155</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>1432.45155</t>
         </is>
       </c>
     </row>
@@ -878,7 +1241,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="A2:D3"/>
@@ -1040,6 +1403,28 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1947.180595</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1947.180595</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>-571</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>-259</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>